<commit_message>
Began work on funnel plots, continuing methods/results writeup
</commit_message>
<xml_diff>
--- a/parsed/Parse_all_results.xlsx
+++ b/parsed/Parse_all_results.xlsx
@@ -18,14 +18,134 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+  <si>
+    <t>studies N</t>
+  </si>
+  <si>
+    <t>Effects N</t>
+  </si>
+  <si>
+    <t>Summary effect</t>
+  </si>
+  <si>
+    <t>Var Effect</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>I2</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>PCF</t>
+  </si>
+  <si>
+    <t>nitrapyrin</t>
+  </si>
+  <si>
+    <t>NBPT</t>
+  </si>
+  <si>
+    <t>NBPT+DCD</t>
+  </si>
+  <si>
+    <t>S.R</t>
+  </si>
+  <si>
+    <t>Urea</t>
+  </si>
+  <si>
+    <t>thiosulfate</t>
+  </si>
+  <si>
+    <t>UAN</t>
+  </si>
+  <si>
+    <t>AA</t>
+  </si>
+  <si>
+    <t>p(Z =/= 0)</t>
+  </si>
+  <si>
+    <t>95% CI</t>
+  </si>
+  <si>
+    <t>Lower limit</t>
+  </si>
+  <si>
+    <t>Upper limit</t>
+  </si>
+  <si>
+    <t>N values</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>Hi</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="3">
+    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="170" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -46,14 +166,47 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="12">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -382,13 +535,540 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:M15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <cols>
+    <col min="4" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>18</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.14430257636528299</v>
+      </c>
+      <c r="E3" s="1">
+        <v>5.2741378241001301E-3</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.160134582574155</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0.371582318776225</v>
+      </c>
+      <c r="H3" s="2">
+        <v>157.53853361860899</v>
+      </c>
+      <c r="I3" s="1">
+        <v>4.6922153175748001E-2</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1.9609876954107498E-3</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.286644165035155</v>
+      </c>
+      <c r="L3" s="1">
+        <v>-1.927</v>
+      </c>
+      <c r="M3" s="1">
+        <v>1.8340000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>31</v>
+      </c>
+      <c r="D4" s="1">
+        <v>5.4450177196288203E-2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5.9342282113064599E-3</v>
+      </c>
+      <c r="F4" s="1">
+        <v>6.1421662251603601E-2</v>
+      </c>
+      <c r="G4" s="7">
+        <v>0.37222818861272799</v>
+      </c>
+      <c r="H4" s="2">
+        <v>47.788064796514099</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.47966990205733601</v>
+      </c>
+      <c r="J4" s="1">
+        <v>-9.6536349012360301E-2</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.205436703404937</v>
+      </c>
+      <c r="L4" s="1">
+        <v>-0.75</v>
+      </c>
+      <c r="M4" s="1">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>39</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.31867036764013501</v>
+      </c>
+      <c r="E5" s="1">
+        <v>9.9836274253130002E-3</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
+      <c r="G5" s="9">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>32.917679848192797</v>
+      </c>
+      <c r="I5" s="1">
+        <v>1.4261008488458699E-3</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0.122830884600881</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0.51450985067939004</v>
+      </c>
+      <c r="L5" s="1">
+        <v>-1.18</v>
+      </c>
+      <c r="M5" s="1">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>62</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.22564454794536401</v>
+      </c>
+      <c r="E6" s="1">
+        <v>8.9014704947577607E-3</v>
+      </c>
+      <c r="F6" s="1">
+        <v>8.4006568069110304E-2</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0.16530526331617301</v>
+      </c>
+      <c r="H6" s="2">
+        <v>73.080609376246898</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1.6773749136347799E-2</v>
+      </c>
+      <c r="J6" s="1">
+        <v>4.0723242918979302E-2</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0.41056585297175002</v>
+      </c>
+      <c r="L6" s="1">
+        <v>-1.7849999999999999</v>
+      </c>
+      <c r="M6" s="1">
+        <v>1.73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>14</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.206451845535775</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1.9523302657723101E-2</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="9">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>11.8467621485993</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0.13952832067996601</v>
+      </c>
+      <c r="J7" s="1">
+        <v>-6.7410746816501596E-2</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0.480314437888051</v>
+      </c>
+      <c r="L7" s="1">
+        <v>-0.45</v>
+      </c>
+      <c r="M7" s="1">
+        <v>2.62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>53</v>
+      </c>
+      <c r="D9" s="1">
+        <v>9.7228450133389599E-2</v>
+      </c>
+      <c r="E9" s="1">
+        <v>4.7051146677437204E-3</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" s="9">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2">
+        <v>30.4428345275516</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0.15635091792295999</v>
+      </c>
+      <c r="J9" s="1">
+        <v>-3.7215473149160599E-2</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0.23167237341593999</v>
+      </c>
+      <c r="L9" s="1">
+        <v>-1.67</v>
+      </c>
+      <c r="M9" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>46</v>
+      </c>
+      <c r="D10" s="1">
+        <v>7.1585109019264098E-2</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1.54147500589349E-2</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.26516628307859702</v>
+      </c>
+      <c r="G10" s="7">
+        <v>0.42873618552677001</v>
+      </c>
+      <c r="H10" s="2">
+        <v>78.772712116371494</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0.564227812064237</v>
+      </c>
+      <c r="J10" s="1">
+        <v>-0.171760948738827</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0.314931166777356</v>
+      </c>
+      <c r="L10" s="1">
+        <v>-1.31</v>
+      </c>
+      <c r="M10" s="1">
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>39</v>
+      </c>
+      <c r="D11" s="1">
+        <v>-0.13168863489163901</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1.2204585819371E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.103209405279983</v>
+      </c>
+      <c r="G11" s="7">
+        <v>0.235895302887142</v>
+      </c>
+      <c r="H11" s="2">
+        <v>49.731404797773898</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0.23324992631091901</v>
+      </c>
+      <c r="J11" s="1">
+        <v>-0.34821839470237598</v>
+      </c>
+      <c r="K11" s="1">
+        <v>8.4841124919098704E-2</v>
+      </c>
+      <c r="L11" s="1">
+        <v>-1.1299999999999999</v>
+      </c>
+      <c r="M11" s="1">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" s="1">
+        <v>-8.3750401606425606E-2</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.16389851079301099</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.103231166666667</v>
+      </c>
+      <c r="G12" s="7">
+        <v>0.29969855324914102</v>
+      </c>
+      <c r="H12" s="2">
+        <v>1.4279564959341899</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0.83611068682352996</v>
+      </c>
+      <c r="J12" s="1">
+        <v>-0.87724426992705296</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0.70974346671420196</v>
+      </c>
+      <c r="L12" s="1">
+        <v>-0.59</v>
+      </c>
+      <c r="M12" s="1">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>14</v>
+      </c>
+      <c r="D13" s="1">
+        <v>-3.0257090714396102E-2</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1.8280170406603902E-2</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13" s="9">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
+        <v>8.9104275227685505</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0.82292216659258099</v>
+      </c>
+      <c r="J13" s="1">
+        <v>-0.29525728436339999</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0.23474310293460801</v>
+      </c>
+      <c r="L13" s="1">
+        <v>-0.53500000000000003</v>
+      </c>
+      <c r="M13" s="1">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="7"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>21</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0.15038657425837801</v>
+      </c>
+      <c r="E15" s="1">
+        <v>6.6799599676808296E-3</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1.53289737437731E-2</v>
+      </c>
+      <c r="G15" s="7">
+        <v>0.11548244910896401</v>
+      </c>
+      <c r="H15" s="2">
+        <v>22.6111963294031</v>
+      </c>
+      <c r="I15" s="1">
+        <v>6.5765554298501797E-2</v>
+      </c>
+      <c r="J15" s="1">
+        <v>-9.8062289877190196E-3</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0.31057937750447501</v>
+      </c>
+      <c r="L15" s="1">
+        <v>-0.5</v>
+      </c>
+      <c r="M15" s="1">
+        <v>1.3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>